<commit_message>
translated korean languages in the file to English
</commit_message>
<xml_diff>
--- a/data/bok_data_download_list.xlsx
+++ b/data/bok_data_download_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dioscuroi/Desktop/BAF507 금융 데이터베이스/exercise/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhkan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C334C5D-7492-C644-874E-BA9388B8EE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C9A90-8257-40BF-9769-E762D32E3850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="3320" windowWidth="26620" windowHeight="13520" xr2:uid="{8D0FA092-C672-B243-9221-812ACBC493A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D0FA092-C672-B243-9221-812ACBC493A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>731Y001</t>
   </si>
   <si>
-    <t>3.1.1.1. 주요국 통화의 대원화환율</t>
-  </si>
-  <si>
     <t>0000001</t>
   </si>
   <si>
@@ -55,21 +52,12 @@
     <t>ITEM_NAME</t>
   </si>
   <si>
-    <t>원/미국달러(매매기준율)</t>
-  </si>
-  <si>
     <t>902Y009</t>
   </si>
   <si>
-    <t>9.1.3.1. 국제 주요국 경상수지</t>
-  </si>
-  <si>
     <t>KR</t>
   </si>
   <si>
-    <t>한국</t>
-  </si>
-  <si>
     <t>CYCLE</t>
   </si>
   <si>
@@ -79,27 +67,15 @@
     <t>D</t>
   </si>
   <si>
-    <t xml:space="preserve">원 </t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
-    <t>백만달러</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
-    <t>미국</t>
-  </si>
-  <si>
     <t>902Y015</t>
   </si>
   <si>
-    <t>9.1.4.1. 국제 주요국 경제성장률</t>
-  </si>
-  <si>
     <t>KOR</t>
   </si>
   <si>
@@ -112,9 +88,6 @@
     <t>902Y016</t>
   </si>
   <si>
-    <t>9.1.4.2. 국제 주요국 국내총생산(GDP)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -124,24 +97,12 @@
     <t>732Y001</t>
   </si>
   <si>
-    <t>3.5. 외환보유액</t>
-  </si>
-  <si>
     <t>99</t>
   </si>
   <si>
-    <t>합계</t>
-  </si>
-  <si>
-    <t xml:space="preserve">천달러 </t>
-  </si>
-  <si>
     <t>902Y008</t>
   </si>
   <si>
-    <t>9.1.2.2. 국제 주요국 소비자물가지수</t>
-  </si>
-  <si>
     <t>2010=100</t>
   </si>
   <si>
@@ -187,30 +148,67 @@
     <t>902Y023</t>
   </si>
   <si>
-    <t>9.1.6.1. 주요국제금리</t>
-  </si>
-  <si>
     <t>IR3TIB</t>
   </si>
   <si>
     <t>ITEM_CODE2</t>
   </si>
   <si>
-    <t>단기금리 - 한국</t>
-  </si>
-  <si>
-    <t>단기금리 - 미국</t>
+    <t>3.1.1.1. Arbitraged Rates of Major Currencies Against Won</t>
+  </si>
+  <si>
+    <t>9.1.2.2. International Consumer Price indices</t>
+  </si>
+  <si>
+    <t>9.1.3.1. Internatioanl Current Account, Total, Net, US Dollars</t>
+  </si>
+  <si>
+    <t>9.1.4.1. International Growth Rate of GDP</t>
+  </si>
+  <si>
+    <t>9.1.4.2. GDP</t>
+  </si>
+  <si>
+    <t>3.5. International Reserves</t>
+  </si>
+  <si>
+    <t>9.1.6.1. Financial Market Key Indicators</t>
+  </si>
+  <si>
+    <t>Won per United States Dollar(Basic Exchange Rate)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korea, Republic Of</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Short term interests rates</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Mil.U$</t>
+  </si>
+  <si>
+    <t>Thou.U$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,7 +216,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -227,6 +225,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,7 +279,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,9 +295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -330,7 +335,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +441,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,7 +583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,325 +593,326 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A0AA41-D8DE-6C4E-BA0D-F6166FFB5BF8}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="A12:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>